<commit_message>
Dynamic Table Program code added
</commit_message>
<xml_diff>
--- a/ProjectWithPOM/src/main/java/Resources/SelectPageTestData.xlsx
+++ b/ProjectWithPOM/src/main/java/Resources/SelectPageTestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aruna\eclipse-workspace\ProjectWithPOM\src\main\java\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5E016-67CF-43AD-8088-7EA604D6036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7385E57-BBFA-462E-8F98-B50B3D236B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{81363341-7362-4BC4-9391-2E61FAFC7659}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{81363341-7362-4BC4-9391-2E61FAFC7659}"/>
   </bookViews>
   <sheets>
     <sheet name="SelectPageTestData" sheetId="1" r:id="rId1"/>
     <sheet name="RadioButtonDemoTestData" sheetId="2" r:id="rId2"/>
+    <sheet name="TableData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Red</t>
   </si>
@@ -58,13 +59,25 @@
   </si>
   <si>
     <t>Radio button 'Female' is checked</t>
+  </si>
+  <si>
+    <t>Herrod Chandler</t>
+  </si>
+  <si>
+    <t>Sales Assistant</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>$137,500</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +93,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,14 +123,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B6A04F-9ED9-4D00-87ED-6C3BB9049ABE}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -485,4 +532,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{343399F0-211C-4DC8-B076-49364C6F146A}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2">
+        <v>59</v>
+      </c>
+      <c r="E1" s="3">
+        <v>41127</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Parameter Passing And Data Provider pgm codes added
</commit_message>
<xml_diff>
--- a/ProjectWithPOM/src/main/java/Resources/SelectPageTestData.xlsx
+++ b/ProjectWithPOM/src/main/java/Resources/SelectPageTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aruna\eclipse-workspace\ProjectWithPOM\src\main\java\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7385E57-BBFA-462E-8F98-B50B3D236B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506FE01B-5378-4B00-9B97-5F1B478D52BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{81363341-7362-4BC4-9391-2E61FAFC7659}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7785" firstSheet="2" activeTab="3" xr2:uid="{81363341-7362-4BC4-9391-2E61FAFC7659}"/>
   </bookViews>
   <sheets>
     <sheet name="SelectPageTestData" sheetId="1" r:id="rId1"/>
     <sheet name="RadioButtonDemoTestData" sheetId="2" r:id="rId2"/>
     <sheet name="TableData" sheetId="3" r:id="rId3"/>
+    <sheet name="FormSubmitByParameter" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Red</t>
   </si>
@@ -71,13 +72,37 @@
   </si>
   <si>
     <t>$137,500</t>
+  </si>
+  <si>
+    <t>Tiger Nixon System Architect Edinburgh 61 2011/04/25 $320,800</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Form has been submitted successfully!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +120,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF212529"/>
       <name val="Times New Roman"/>
@@ -115,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -138,19 +169,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEE2E6"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -499,9 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B6A04F-9ED9-4D00-87ED-6C3BB9049ABE}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -536,40 +583,94 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{343399F0-211C-4DC8-B076-49364C6F146A}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D2" s="3">
         <v>59</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E2" s="4">
         <v>41127</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61024F5F-A1B4-41F9-9847-C96B750CB4BB}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>